<commit_message>
cca - chapter 5
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA95C430-AC1E-43E0-8DC3-30020FA9BD35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB314379-42C5-4ECB-8ED0-CADBA3007D66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
   <si>
     <t>"&gt;</t>
   </si>
@@ -157,14 +157,6 @@
 --password itversity</t>
   </si>
   <si>
-    <t>sqoop import \
---connect jdbc:mysql://ms.itversity.com:3306/retail_db \
---username retail_user \
---password itversity \
---table order \
---target-dir /user/training/sqoop_import/retail_db/orders</t>
-  </si>
-  <si>
     <t>Redirect sqoop logs</t>
   </si>
   <si>
@@ -174,12 +166,58 @@
 --password itversity \
 --query "SELECT * FROM orders LIMIT 10" 1&gt;query.out 2&gt;query.err</t>
   </si>
+  <si>
+    <t>5. Sqoop -Importing data into HDFS</t>
+  </si>
+  <si>
+    <t>sqoop import \
+--connect jdbc:mysql://ms.itversity.com:3306/retail_db \
+--username retail_user \
+--password itversity \
+--table order_items \
+--warehouse-dir /user/neogia01/sqoop_import/retail_db</t>
+  </si>
+  <si>
+    <t>Sqoop import  target-dir</t>
+  </si>
+  <si>
+    <t>Sqoop import warehouse-dir</t>
+  </si>
+  <si>
+    <t>sqoop import \
+--connect jdbc:mysql://ms.itversity.com:3306/retail_db \
+--username retail_user \
+--password itversity \
+--table orders \
+--target-dir /user/neogia01/sqoop_import/retail_db/orders \</t>
+  </si>
+  <si>
+    <t>sqoop import \
+--connect jdbc:mysql://ms.itversity.com:3306/retail_db \
+--username retail_user \
+--password itversity \
+--table order_items \
+--warehouse-dir /user/neogia01/sqoop_import/retail_db \
+--append</t>
+  </si>
+  <si>
+    <t>sqoop import \
+--connect jdbc:mysql://ms.itversity.com:3306/retail_db \
+--username retail_user \
+--password itversity \
+--table order_items \
+--warehouse-dir /user/neogia01/sqoop_import/retail_db \
+--delete-target-dir</t>
+  </si>
+  <si>
+    <t>Sqoop import - append/delete</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,7 +272,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -410,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -427,47 +472,56 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1536,52 +1590,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399CFA12-9C70-4F6A-B463-E5E2CF5BBC49}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="50.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.21875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="53.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="50.77734375" style="6"/>
+    <col min="1" max="1" width="49.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="50.77734375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1589,35 +1643,70 @@
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cca - chapter 5 - 2
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB314379-42C5-4ECB-8ED0-CADBA3007D66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B762F89D-7D1B-4E3B-8CB1-72C93E53D382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="31">
   <si>
     <t>"&gt;</t>
   </si>
@@ -178,12 +178,6 @@
 --warehouse-dir /user/neogia01/sqoop_import/retail_db</t>
   </si>
   <si>
-    <t>Sqoop import  target-dir</t>
-  </si>
-  <si>
-    <t>Sqoop import warehouse-dir</t>
-  </si>
-  <si>
     <t>sqoop import \
 --connect jdbc:mysql://ms.itversity.com:3306/retail_db \
 --username retail_user \
@@ -210,7 +204,29 @@
 --delete-target-dir</t>
   </si>
   <si>
-    <t>Sqoop import - append/delete</t>
+    <t>sqoop import \
+--connect jdbc:mysql://ms.itversity.com:3306/retail_db \
+--username retail_user \
+--password itversity \
+--table order_items \
+--warehouse-dir /user/neogia01/sqoop_import/retail_db \
+--delete-target-dir
+--num-mappers 8</t>
+  </si>
+  <si>
+    <t>Sqoop import - append</t>
+  </si>
+  <si>
+    <t>Sqoop import - delete</t>
+  </si>
+  <si>
+    <t>Sqoop import - target-dir</t>
+  </si>
+  <si>
+    <t>Sqoop import - warehouse-dir</t>
+  </si>
+  <si>
+    <t>Sqoop import - num-mappers</t>
   </si>
 </sst>
 </file>
@@ -455,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -472,6 +488,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -481,18 +524,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -502,26 +533,17 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1590,123 +1612,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399CFA12-9C70-4F6A-B463-E5E2CF5BBC49}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="50.77734375" style="9"/>
+    <col min="1" max="1" width="49.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="50.77734375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="21"/>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="16" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
formatting + chapter 10
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCodes\github\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29992466-11E9-42ED-BD04-913D4210CACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE8C560-BBBE-4391-B5DB-4A3D990E146F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -20,12 +20,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">schedule!$A$1:$N$19</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -803,6 +802,57 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -826,143 +876,13 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1299,223 +1219,223 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="28">
-        <v>1</v>
-      </c>
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="22">
         <v>15</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="22">
         <v>15</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="28" t="str">
+      <c r="F2" s="20" t="str">
         <f>IF(C2=D2,"Completed",IF(C2=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="28">
-        <v>2</v>
-      </c>
-      <c r="B3" s="29" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="22">
         <v>8</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="22">
         <v>8</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="28" t="str">
+      <c r="F3" s="20" t="str">
         <f t="shared" ref="F3:F9" si="0">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="22">
         <v>10</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="22">
         <v>10</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="28" t="str">
+      <c r="F4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Completed</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="22">
         <v>10</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="22">
         <v>10</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="28" t="str">
+      <c r="F5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Completed</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
         <v>5</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="22">
         <v>11</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="22">
         <v>11</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="28" t="str">
+      <c r="F6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Completed</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="28">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="22">
         <v>14</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="22">
         <v>14</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="28" t="str">
+      <c r="F7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Completed</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="28">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
         <v>7</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="22">
         <v>11</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="22">
         <v>11</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="28" t="str">
+      <c r="F8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Completed</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="28">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="22">
         <v>14</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="22">
         <v>14</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="28" t="str">
+      <c r="F9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Completed</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="33">
-        <v>0</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="C10" s="25">
+        <v>0</v>
+      </c>
+      <c r="D10" s="25">
         <v>13</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="31" t="str">
+      <c r="F10" s="23" t="str">
         <f t="shared" ref="F10:F19" si="1">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
         <v>Not Started</v>
       </c>
@@ -1524,213 +1444,213 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
         <v>10</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="38">
-        <v>6</v>
-      </c>
-      <c r="D11" s="38">
+      <c r="C11" s="29">
+        <v>7</v>
+      </c>
+      <c r="D11" s="29">
         <v>44</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="36" t="str">
+      <c r="F11" s="27" t="str">
         <f t="shared" si="1"/>
         <v>In Progress</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="31">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="33">
-        <v>0</v>
-      </c>
-      <c r="D12" s="33">
+      <c r="C12" s="25">
+        <v>0</v>
+      </c>
+      <c r="D12" s="25">
         <v>12</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="31" t="str">
+      <c r="F12" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="39">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
         <v>12</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="41">
-        <v>0</v>
-      </c>
-      <c r="D13" s="41">
+      <c r="C13" s="32">
+        <v>0</v>
+      </c>
+      <c r="D13" s="32">
         <v>21</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="39" t="str">
+      <c r="F13" s="30" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="31">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="33">
-        <v>0</v>
-      </c>
-      <c r="D14" s="33">
+      <c r="C14" s="25">
+        <v>0</v>
+      </c>
+      <c r="D14" s="25">
         <v>9</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="31" t="str">
+      <c r="F14" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="31">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
         <v>14</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="33">
-        <v>0</v>
-      </c>
-      <c r="D15" s="33">
+      <c r="C15" s="25">
+        <v>0</v>
+      </c>
+      <c r="D15" s="25">
         <v>8</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="31" t="str">
+      <c r="F15" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="31">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
         <v>15</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="33">
-        <v>0</v>
-      </c>
-      <c r="D16" s="33">
+      <c r="C16" s="25">
+        <v>0</v>
+      </c>
+      <c r="D16" s="25">
         <v>7</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="31" t="str">
+      <c r="F16" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="31">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
         <v>16</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="33">
-        <v>0</v>
-      </c>
-      <c r="D17" s="33">
+      <c r="C17" s="25">
+        <v>0</v>
+      </c>
+      <c r="D17" s="25">
         <v>7</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="31" t="str">
+      <c r="F17" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="39">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="30">
         <v>17</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="41">
-        <v>0</v>
-      </c>
-      <c r="D18" s="41">
+      <c r="C18" s="32">
+        <v>0</v>
+      </c>
+      <c r="D18" s="32">
         <v>27</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="39" t="str">
+      <c r="F18" s="30" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="31">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
         <v>18</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="33">
-        <v>0</v>
-      </c>
-      <c r="D19" s="33">
+      <c r="C19" s="25">
+        <v>0</v>
+      </c>
+      <c r="D19" s="25">
         <v>8</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="31" t="str">
+      <c r="F19" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Not Started</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="34">
+      <c r="B20" s="33"/>
+      <c r="C20" s="26">
         <f>SUM(C2:C19)</f>
-        <v>99</v>
-      </c>
-      <c r="D20" s="34">
+        <v>100</v>
+      </c>
+      <c r="D20" s="26">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="33">
         <f>ROUND(C20*100/D20,0)</f>
         <v>40</v>
       </c>
-      <c r="F20" s="35"/>
+      <c r="F20" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N19" xr:uid="{D3CEC666-E820-4D85-92B5-084C9F56284E}"/>
@@ -1751,26 +1671,26 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="71.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="45.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="92.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="140.6640625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="4"/>
-    <col min="10" max="10" width="52.44140625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="92.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="140.7109375" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" style="4"/>
+    <col min="10" max="10" width="52.42578125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1796,7 +1716,7 @@
         <v>&lt;a href="http://discuss.itversity.com/t/introduction-cca-175-spark-and-hadoop-developer-curriculum/19794" target="_blank"&gt;http://discuss.itversity.com/t/introduction-cca-175-spark-and-hadoop-developer-curriculum/19794&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1819,7 +1739,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1842,7 +1762,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +1785,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1888,7 +1808,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1911,7 +1831,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1934,7 +1854,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1957,7 +1877,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1980,7 +1900,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2003,7 +1923,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2026,7 +1946,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2049,7 +1969,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2072,7 +1992,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2095,7 +2015,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2118,7 +2038,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2141,7 +2061,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2164,7 +2084,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2187,7 +2107,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2210,7 +2130,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2233,7 +2153,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2256,7 +2176,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2279,7 +2199,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2302,7 +2222,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -2325,7 +2245,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2348,7 +2268,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2291,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2394,7 +2314,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -2417,7 +2337,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2440,7 +2360,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2477,24 +2397,24 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="50.6640625" style="6"/>
+    <col min="1" max="1" width="49.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="50.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2508,7 +2428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
@@ -2522,17 +2442,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -2546,16 +2466,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="35"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -2569,7 +2489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -2583,7 +2503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -2597,7 +2517,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2611,7 +2531,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2623,7 +2543,7 @@
       </c>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>37</v>
       </c>
@@ -2635,16 +2555,16 @@
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="35"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -2652,7 +2572,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
chapter 12 - 1
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27A2059-A9BD-4E0E-B722-2832E04E4E19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6DA187-B066-47FA-94EE-25215F0FA07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="93">
   <si>
     <t>"&gt;</t>
   </si>
@@ -459,6 +459,18 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>total minutes</t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -575,12 +587,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -748,12 +760,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -833,6 +854,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -842,15 +881,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -877,6 +907,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1217,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444F08F4-42AE-4713-B59A-E734A31EF081}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="K13" sqref="K13:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,9 +1269,11 @@
     <col min="3" max="4" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -1251,8 +1292,20 @@
       <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H1" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1272,8 +1325,22 @@
         <f>IF(C2=D2,"Completed",IF(C2=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H2" s="46">
+        <v>1</v>
+      </c>
+      <c r="I2" s="46">
+        <v>6</v>
+      </c>
+      <c r="J2" s="46">
+        <f t="shared" ref="J2:J9" si="0">H2*60+I2</f>
+        <v>66</v>
+      </c>
+      <c r="K2" s="46">
+        <f t="shared" ref="K2:K9" si="1">ROUND(J2/D2,2)</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1290,11 +1357,25 @@
         <v>53</v>
       </c>
       <c r="F3" s="20" t="str">
-        <f t="shared" ref="F3:F9" si="0">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
+        <f t="shared" ref="F3:F9" si="2">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="46">
+        <v>1</v>
+      </c>
+      <c r="I3" s="46">
+        <v>39</v>
+      </c>
+      <c r="J3" s="46">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="K3" s="46">
+        <f t="shared" si="1"/>
+        <v>12.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -1311,11 +1392,25 @@
         <v>55</v>
       </c>
       <c r="F4" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H4" s="46">
+        <v>1</v>
+      </c>
+      <c r="I4" s="46">
+        <v>33</v>
+      </c>
+      <c r="J4" s="46">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="K4" s="46">
+        <f t="shared" si="1"/>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -1332,11 +1427,25 @@
         <v>57</v>
       </c>
       <c r="F5" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H5" s="46">
+        <v>0</v>
+      </c>
+      <c r="I5" s="46">
+        <v>37</v>
+      </c>
+      <c r="J5" s="46">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="K5" s="46">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>5</v>
       </c>
@@ -1353,11 +1462,25 @@
         <v>59</v>
       </c>
       <c r="F6" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H6" s="46">
+        <v>0</v>
+      </c>
+      <c r="I6" s="46">
+        <v>52</v>
+      </c>
+      <c r="J6" s="46">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="K6" s="46">
+        <f t="shared" si="1"/>
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -1374,11 +1497,25 @@
         <v>61</v>
       </c>
       <c r="F7" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H7" s="46">
+        <v>1</v>
+      </c>
+      <c r="I7" s="46">
+        <v>14</v>
+      </c>
+      <c r="J7" s="46">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="K7" s="46">
+        <f t="shared" si="1"/>
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -1395,11 +1532,25 @@
         <v>63</v>
       </c>
       <c r="F8" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H8" s="46">
+        <v>0</v>
+      </c>
+      <c r="I8" s="46">
+        <v>50</v>
+      </c>
+      <c r="J8" s="46">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K8" s="46">
+        <f t="shared" si="1"/>
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>8</v>
       </c>
@@ -1416,11 +1567,25 @@
         <v>65</v>
       </c>
       <c r="F9" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H9" s="46">
+        <v>1</v>
+      </c>
+      <c r="I9" s="46">
+        <v>16</v>
+      </c>
+      <c r="J9" s="46">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="K9" s="46">
+        <f t="shared" si="1"/>
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -1437,78 +1602,130 @@
         <v>67</v>
       </c>
       <c r="F10" s="23" t="str">
-        <f t="shared" ref="F10:F19" si="1">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
+        <f t="shared" ref="F10:F19" si="3">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
         <v>Not Started</v>
       </c>
-      <c r="J10">
-        <f>44+21+27</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
+      <c r="H10" s="46">
+        <v>0</v>
+      </c>
+      <c r="I10" s="46">
+        <v>47</v>
+      </c>
+      <c r="J10" s="46">
+        <f>H10*60+I10</f>
+        <v>47</v>
+      </c>
+      <c r="K10" s="46">
+        <f>ROUND(J10/D10,2)</f>
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="29">
-        <v>19</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="C11" s="32">
         <v>44</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="D11" s="32">
+        <v>44</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F11" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>Completed</v>
+      </c>
+      <c r="H11" s="46">
+        <v>5</v>
+      </c>
+      <c r="I11" s="46">
+        <v>47</v>
+      </c>
+      <c r="J11" s="46">
+        <f>H11*60+I11</f>
+        <v>347</v>
+      </c>
+      <c r="K11" s="46">
+        <f t="shared" ref="K11:K19" si="4">ROUND(J11/D11,2)</f>
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
+        <v>11</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="22">
+        <v>12</v>
+      </c>
+      <c r="D12" s="22">
+        <v>12</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>Completed</v>
+      </c>
+      <c r="H12" s="46">
+        <v>1</v>
+      </c>
+      <c r="I12" s="46">
+        <v>35</v>
+      </c>
+      <c r="J12" s="46">
+        <f t="shared" ref="J12:J19" si="5">H12*60+I12</f>
+        <v>95</v>
+      </c>
+      <c r="K12" s="46">
+        <f t="shared" si="4"/>
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="33">
+        <v>12</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="35">
+        <v>1</v>
+      </c>
+      <c r="D13" s="35">
+        <v>21</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="33" t="str">
+        <f t="shared" si="3"/>
         <v>In Progress</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="23">
-        <v>11</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="25">
-        <v>0</v>
-      </c>
-      <c r="D12" s="25">
-        <v>12</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>Not Started</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
-        <v>12</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="32">
-        <v>0</v>
-      </c>
-      <c r="D13" s="32">
-        <v>21</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v>Not Started</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H13" s="46">
+        <v>4</v>
+      </c>
+      <c r="I13" s="46">
+        <v>6</v>
+      </c>
+      <c r="J13" s="46">
+        <f t="shared" si="5"/>
+        <v>246</v>
+      </c>
+      <c r="K13" s="46">
+        <f t="shared" si="4"/>
+        <v>11.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -1525,11 +1742,25 @@
         <v>75</v>
       </c>
       <c r="F14" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H14" s="46">
+        <v>1</v>
+      </c>
+      <c r="I14" s="46">
+        <v>34</v>
+      </c>
+      <c r="J14" s="46">
+        <f t="shared" si="5"/>
+        <v>94</v>
+      </c>
+      <c r="K14" s="46">
+        <f t="shared" si="4"/>
+        <v>10.44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -1546,11 +1777,25 @@
         <v>77</v>
       </c>
       <c r="F15" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H15" s="46">
+        <v>1</v>
+      </c>
+      <c r="I15" s="46">
+        <v>12</v>
+      </c>
+      <c r="J15" s="46">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="K15" s="46">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -1567,11 +1812,25 @@
         <v>79</v>
       </c>
       <c r="F16" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H16" s="46">
+        <v>1</v>
+      </c>
+      <c r="I16" s="46">
+        <v>20</v>
+      </c>
+      <c r="J16" s="46">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="K16" s="46">
+        <f t="shared" si="4"/>
+        <v>11.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -1588,32 +1847,60 @@
         <v>81</v>
       </c>
       <c r="F17" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="30">
+      <c r="H17" s="46">
+        <v>0</v>
+      </c>
+      <c r="I17" s="46">
+        <v>53</v>
+      </c>
+      <c r="J17" s="46">
+        <f t="shared" si="5"/>
+        <v>53</v>
+      </c>
+      <c r="K17" s="46">
+        <f t="shared" si="4"/>
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="27">
         <v>17</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="32">
-        <v>0</v>
-      </c>
-      <c r="D18" s="32">
+      <c r="C18" s="29">
+        <v>0</v>
+      </c>
+      <c r="D18" s="29">
         <v>27</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="30" t="str">
-        <f t="shared" si="1"/>
+      <c r="F18" s="27" t="str">
+        <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H18" s="46">
+        <v>4</v>
+      </c>
+      <c r="I18" s="46">
+        <v>14</v>
+      </c>
+      <c r="J18" s="46">
+        <f t="shared" si="5"/>
+        <v>254</v>
+      </c>
+      <c r="K18" s="46">
+        <f t="shared" si="4"/>
+        <v>9.41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -1630,28 +1917,42 @@
         <v>85</v>
       </c>
       <c r="F19" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="H19" s="46">
+        <v>1</v>
+      </c>
+      <c r="I19" s="46">
+        <v>0</v>
+      </c>
+      <c r="J19" s="46">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="K19" s="46">
+        <f t="shared" si="4"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="26">
         <f>SUM(C2:C19)</f>
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="D20" s="26">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="36">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>45</v>
-      </c>
-      <c r="F20" s="33"/>
+        <v>60</v>
+      </c>
+      <c r="F20" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N19" xr:uid="{D3CEC666-E820-4D85-92B5-084C9F56284E}"/>
@@ -2408,12 +2709,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2444,11 +2745,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2469,12 +2770,12 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -2558,12 +2859,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>

<commit_message>
chapter 12 - 3
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61FFD5A-0AE2-4417-99ED-63CB32562858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0665D08A-B663-4DA1-A9FC-8E960F61162F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,7 +1698,7 @@
         <v>72</v>
       </c>
       <c r="C13" s="35">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D13" s="35">
         <v>21</v>
@@ -1942,7 +1942,7 @@
       <c r="B20" s="39"/>
       <c r="C20" s="26">
         <f>SUM(C2:C19)</f>
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D20" s="26">
         <f>SUM(D2:D19)</f>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E20" s="39">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F20" s="39"/>
     </row>

</xml_diff>

<commit_message>
chapter 12 - 4
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0665D08A-B663-4DA1-A9FC-8E960F61162F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF807F65-B1BA-45C1-B0DE-B088BE276834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1698,7 +1698,7 @@
         <v>72</v>
       </c>
       <c r="C13" s="35">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D13" s="35">
         <v>21</v>
@@ -1942,7 +1942,7 @@
       <c r="B20" s="39"/>
       <c r="C20" s="26">
         <f>SUM(C2:C19)</f>
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D20" s="26">
         <f>SUM(D2:D19)</f>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E20" s="39">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F20" s="39"/>
     </row>

</xml_diff>

<commit_message>
chapter 17 - 1
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF807F65-B1BA-45C1-B0DE-B088BE276834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753591CA-86DD-4593-8118-D4FE055ED62F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -470,14 +470,14 @@
     <t>total minutes</t>
   </si>
   <si>
-    <t>average</t>
+    <t>Average mins per Topic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,8 +553,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,6 +632,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -774,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -854,15 +901,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -890,9 +928,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -916,6 +951,44 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1259,7 +1332,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1269,8 +1342,9 @@
     <col min="3" max="4" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" customWidth="1"/>
+    <col min="7" max="9" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1292,16 +1366,16 @@
       <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="47" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1325,17 +1399,17 @@
         <f>IF(C2=D2,"Completed",IF(C2=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H2" s="37">
-        <v>1</v>
-      </c>
-      <c r="I2" s="37">
+      <c r="H2" s="34">
+        <v>1</v>
+      </c>
+      <c r="I2" s="34">
         <v>6</v>
       </c>
-      <c r="J2" s="37">
+      <c r="J2" s="34">
         <f t="shared" ref="J2:J9" si="0">H2*60+I2</f>
         <v>66</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="48">
         <f t="shared" ref="K2:K9" si="1">ROUND(J2/D2,2)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -1360,17 +1434,17 @@
         <f t="shared" ref="F3:F9" si="2">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H3" s="37">
-        <v>1</v>
-      </c>
-      <c r="I3" s="37">
+      <c r="H3" s="34">
+        <v>1</v>
+      </c>
+      <c r="I3" s="34">
         <v>39</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="34">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="48">
         <f t="shared" si="1"/>
         <v>12.38</v>
       </c>
@@ -1395,17 +1469,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H4" s="37">
-        <v>1</v>
-      </c>
-      <c r="I4" s="37">
+      <c r="H4" s="34">
+        <v>1</v>
+      </c>
+      <c r="I4" s="34">
         <v>33</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="34">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="48">
         <f t="shared" si="1"/>
         <v>9.3000000000000007</v>
       </c>
@@ -1430,17 +1504,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H5" s="37">
-        <v>0</v>
-      </c>
-      <c r="I5" s="37">
+      <c r="H5" s="34">
+        <v>0</v>
+      </c>
+      <c r="I5" s="34">
         <v>37</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="34">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="48">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
@@ -1465,17 +1539,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H6" s="37">
-        <v>0</v>
-      </c>
-      <c r="I6" s="37">
+      <c r="H6" s="34">
+        <v>0</v>
+      </c>
+      <c r="I6" s="34">
         <v>52</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="34">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="48">
         <f t="shared" si="1"/>
         <v>4.7300000000000004</v>
       </c>
@@ -1500,17 +1574,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H7" s="37">
-        <v>1</v>
-      </c>
-      <c r="I7" s="37">
+      <c r="H7" s="34">
+        <v>1</v>
+      </c>
+      <c r="I7" s="34">
         <v>14</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="34">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="48">
         <f t="shared" si="1"/>
         <v>5.29</v>
       </c>
@@ -1535,17 +1609,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H8" s="37">
-        <v>0</v>
-      </c>
-      <c r="I8" s="37">
+      <c r="H8" s="34">
+        <v>0</v>
+      </c>
+      <c r="I8" s="34">
         <v>50</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="34">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="48">
         <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
@@ -1570,17 +1644,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H9" s="37">
-        <v>1</v>
-      </c>
-      <c r="I9" s="37">
+      <c r="H9" s="34">
+        <v>1</v>
+      </c>
+      <c r="I9" s="34">
         <v>16</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="34">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="48">
         <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
@@ -1605,52 +1679,52 @@
         <f t="shared" ref="F10:F19" si="3">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
         <v>Not Started</v>
       </c>
-      <c r="H10" s="37">
-        <v>0</v>
-      </c>
-      <c r="I10" s="37">
+      <c r="H10" s="34">
+        <v>0</v>
+      </c>
+      <c r="I10" s="34">
         <v>47</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="34">
         <f>H10*60+I10</f>
         <v>47</v>
       </c>
-      <c r="K10" s="37">
+      <c r="K10" s="49">
         <f>ROUND(J10/D10,2)</f>
         <v>3.62</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="27">
         <v>10</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="29">
         <v>44</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="29">
         <v>44</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="30" t="str">
+      <c r="F11" s="27" t="str">
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="34">
         <v>5</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="34">
         <v>47</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="34">
         <f>H11*60+I11</f>
         <v>347</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="48">
         <f t="shared" ref="K11:K19" si="4">ROUND(J11/D11,2)</f>
         <v>7.89</v>
       </c>
@@ -1675,52 +1749,52 @@
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H12" s="37">
-        <v>1</v>
-      </c>
-      <c r="I12" s="37">
+      <c r="H12" s="34">
+        <v>1</v>
+      </c>
+      <c r="I12" s="34">
         <v>35</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="34">
         <f t="shared" ref="J12:J19" si="5">H12*60+I12</f>
         <v>95</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="48">
         <f t="shared" si="4"/>
         <v>7.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="33">
+      <c r="A13" s="44">
         <v>12</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="35">
-        <v>16</v>
-      </c>
-      <c r="D13" s="35">
+      <c r="C13" s="46">
         <v>21</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="D13" s="46">
+        <v>21</v>
+      </c>
+      <c r="E13" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="33" t="str">
+      <c r="F13" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>In Progress</v>
-      </c>
-      <c r="H13" s="37">
+        <v>Completed</v>
+      </c>
+      <c r="H13" s="34">
         <v>4</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="34">
         <v>6</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="34">
         <f t="shared" si="5"/>
         <v>246</v>
       </c>
-      <c r="K13" s="37">
+      <c r="K13" s="48">
         <f t="shared" si="4"/>
         <v>11.71</v>
       </c>
@@ -1745,17 +1819,17 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H14" s="37">
-        <v>1</v>
-      </c>
-      <c r="I14" s="37">
+      <c r="H14" s="34">
+        <v>1</v>
+      </c>
+      <c r="I14" s="34">
         <v>34</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="34">
         <f t="shared" si="5"/>
         <v>94</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="49">
         <f t="shared" si="4"/>
         <v>10.44</v>
       </c>
@@ -1780,17 +1854,17 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H15" s="37">
-        <v>1</v>
-      </c>
-      <c r="I15" s="37">
+      <c r="H15" s="34">
+        <v>1</v>
+      </c>
+      <c r="I15" s="34">
         <v>12</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15" s="34">
         <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="K15" s="37">
+      <c r="K15" s="49">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
@@ -1815,17 +1889,17 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H16" s="37">
-        <v>1</v>
-      </c>
-      <c r="I16" s="37">
+      <c r="H16" s="34">
+        <v>1</v>
+      </c>
+      <c r="I16" s="34">
         <v>20</v>
       </c>
-      <c r="J16" s="37">
+      <c r="J16" s="34">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="K16" s="37">
+      <c r="K16" s="49">
         <f t="shared" si="4"/>
         <v>11.43</v>
       </c>
@@ -1850,52 +1924,53 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H17" s="37">
-        <v>0</v>
-      </c>
-      <c r="I17" s="37">
+      <c r="H17" s="34">
+        <v>0</v>
+      </c>
+      <c r="I17" s="34">
         <v>53</v>
       </c>
-      <c r="J17" s="37">
+      <c r="J17" s="34">
         <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="K17" s="37">
+      <c r="K17" s="49">
         <f t="shared" si="4"/>
         <v>7.57</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="30">
         <v>17</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="29">
-        <v>0</v>
-      </c>
-      <c r="D18" s="29">
+      <c r="C18" s="32">
+        <v>2</v>
+      </c>
+      <c r="D18" s="32">
         <v>27</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="27" t="str">
+      <c r="F18" s="30" t="str">
         <f t="shared" si="3"/>
-        <v>Not Started</v>
-      </c>
-      <c r="H18" s="37">
+        <v>In Progress</v>
+      </c>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56">
         <v>4</v>
       </c>
-      <c r="I18" s="37">
+      <c r="I18" s="56">
         <v>14</v>
       </c>
-      <c r="J18" s="37">
+      <c r="J18" s="56">
         <f t="shared" si="5"/>
         <v>254</v>
       </c>
-      <c r="K18" s="37">
+      <c r="K18" s="57">
         <f t="shared" si="4"/>
         <v>9.41</v>
       </c>
@@ -1920,39 +1995,50 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H19" s="37">
-        <v>1</v>
-      </c>
-      <c r="I19" s="37">
-        <v>0</v>
-      </c>
-      <c r="J19" s="37">
+      <c r="H19" s="34">
+        <v>1</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0</v>
+      </c>
+      <c r="J19" s="34">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="K19" s="37">
-        <f t="shared" si="4"/>
+      <c r="K19" s="49">
+        <f>ROUND(J19/D19,2)</f>
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="26">
+      <c r="B20" s="50"/>
+      <c r="C20" s="51">
         <f>SUM(C2:C19)</f>
-        <v>165</v>
-      </c>
-      <c r="D20" s="26">
+        <v>172</v>
+      </c>
+      <c r="D20" s="51">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="50">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>66</v>
-      </c>
-      <c r="F20" s="39"/>
+        <v>69</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="53">
+        <f>SUM(J2:J19)</f>
+        <v>1895</v>
+      </c>
+      <c r="K20" s="54">
+        <f>ROUND(J20/D20,2)</f>
+        <v>7.61</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N19" xr:uid="{D3CEC666-E820-4D85-92B5-084C9F56284E}"/>
@@ -2709,12 +2795,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2745,11 +2831,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2770,12 +2856,12 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -2859,12 +2945,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>

<commit_message>
chapter 17 - 2
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753591CA-86DD-4593-8118-D4FE055ED62F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11F6FDB-DF43-405B-BD12-9B459387616D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -928,30 +928,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -968,9 +944,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -989,6 +962,33 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1375,7 +1375,7 @@
       <c r="J1" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="39" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1409,7 +1409,7 @@
         <f t="shared" ref="J2:J9" si="0">H2*60+I2</f>
         <v>66</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="40">
         <f t="shared" ref="K2:K9" si="1">ROUND(J2/D2,2)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -1444,7 +1444,7 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="K3" s="48">
+      <c r="K3" s="40">
         <f t="shared" si="1"/>
         <v>12.38</v>
       </c>
@@ -1479,7 +1479,7 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="K4" s="48">
+      <c r="K4" s="40">
         <f t="shared" si="1"/>
         <v>9.3000000000000007</v>
       </c>
@@ -1514,7 +1514,7 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K5" s="48">
+      <c r="K5" s="40">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
@@ -1549,7 +1549,7 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="K6" s="48">
+      <c r="K6" s="40">
         <f t="shared" si="1"/>
         <v>4.7300000000000004</v>
       </c>
@@ -1584,7 +1584,7 @@
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="K7" s="48">
+      <c r="K7" s="40">
         <f t="shared" si="1"/>
         <v>5.29</v>
       </c>
@@ -1619,7 +1619,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K8" s="48">
+      <c r="K8" s="40">
         <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
@@ -1654,7 +1654,7 @@
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="K9" s="48">
+      <c r="K9" s="40">
         <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
@@ -1689,7 +1689,7 @@
         <f>H10*60+I10</f>
         <v>47</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="41">
         <f>ROUND(J10/D10,2)</f>
         <v>3.62</v>
       </c>
@@ -1724,8 +1724,8 @@
         <f>H11*60+I11</f>
         <v>347</v>
       </c>
-      <c r="K11" s="48">
-        <f t="shared" ref="K11:K19" si="4">ROUND(J11/D11,2)</f>
+      <c r="K11" s="40">
+        <f t="shared" ref="K11:K18" si="4">ROUND(J11/D11,2)</f>
         <v>7.89</v>
       </c>
     </row>
@@ -1759,28 +1759,28 @@
         <f t="shared" ref="J12:J19" si="5">H12*60+I12</f>
         <v>95</v>
       </c>
-      <c r="K12" s="48">
+      <c r="K12" s="40">
         <f t="shared" si="4"/>
         <v>7.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="44">
+      <c r="A13" s="36">
         <v>12</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="38">
         <v>21</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="38">
         <v>21</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="44" t="str">
+      <c r="F13" s="36" t="str">
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
@@ -1794,7 +1794,7 @@
         <f t="shared" si="5"/>
         <v>246</v>
       </c>
-      <c r="K13" s="48">
+      <c r="K13" s="40">
         <f t="shared" si="4"/>
         <v>11.71</v>
       </c>
@@ -1829,7 +1829,7 @@
         <f t="shared" si="5"/>
         <v>94</v>
       </c>
-      <c r="K14" s="49">
+      <c r="K14" s="41">
         <f t="shared" si="4"/>
         <v>10.44</v>
       </c>
@@ -1864,7 +1864,7 @@
         <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="K15" s="49">
+      <c r="K15" s="41">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
@@ -1899,7 +1899,7 @@
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="K16" s="49">
+      <c r="K16" s="41">
         <f t="shared" si="4"/>
         <v>11.43</v>
       </c>
@@ -1934,7 +1934,7 @@
         <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="K17" s="49">
+      <c r="K17" s="41">
         <f t="shared" si="4"/>
         <v>7.57</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D18" s="32">
         <v>27</v>
@@ -1959,18 +1959,18 @@
         <f t="shared" si="3"/>
         <v>In Progress</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56">
+      <c r="G18" s="46"/>
+      <c r="H18" s="47">
         <v>4</v>
       </c>
-      <c r="I18" s="56">
+      <c r="I18" s="47">
         <v>14</v>
       </c>
-      <c r="J18" s="56">
+      <c r="J18" s="47">
         <f t="shared" si="5"/>
         <v>254</v>
       </c>
-      <c r="K18" s="57">
+      <c r="K18" s="48">
         <f t="shared" si="4"/>
         <v>9.41</v>
       </c>
@@ -2005,37 +2005,37 @@
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="K19" s="49">
+      <c r="K19" s="41">
         <f>ROUND(J19/D19,2)</f>
         <v>7.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51">
+      <c r="B20" s="49"/>
+      <c r="C20" s="42">
         <f>SUM(C2:C19)</f>
-        <v>172</v>
-      </c>
-      <c r="D20" s="51">
+        <v>176</v>
+      </c>
+      <c r="D20" s="42">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="49">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>69</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="53">
+        <v>71</v>
+      </c>
+      <c r="F20" s="49"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="44">
         <f>SUM(J2:J19)</f>
         <v>1895</v>
       </c>
-      <c r="K20" s="54">
+      <c r="K20" s="45">
         <f>ROUND(J20/D20,2)</f>
         <v>7.61</v>
       </c>
@@ -2795,12 +2795,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="52"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2831,11 +2831,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2856,12 +2856,12 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -2945,12 +2945,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>

<commit_message>
chapter 17 - 3
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11F6FDB-DF43-405B-BD12-9B459387616D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9788D4C0-FA45-4A63-9439-A356B177A307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,7 +1947,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="32">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D18" s="32">
         <v>27</v>
@@ -2017,7 +2017,7 @@
       <c r="B20" s="49"/>
       <c r="C20" s="42">
         <f>SUM(C2:C19)</f>
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D20" s="42">
         <f>SUM(D2:D19)</f>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="E20" s="49">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="43"/>

</xml_diff>

<commit_message>
chapter 17 - 4
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9788D4C0-FA45-4A63-9439-A356B177A307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51253FB3-C75E-406D-A7A7-2C27C91EA401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,7 +1947,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="32">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D18" s="32">
         <v>27</v>
@@ -2017,7 +2017,7 @@
       <c r="B20" s="49"/>
       <c r="C20" s="42">
         <f>SUM(C2:C19)</f>
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D20" s="42">
         <f>SUM(D2:D19)</f>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="E20" s="49">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="43"/>

</xml_diff>

<commit_message>
chapter 17 - 5
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCodes\github\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51253FB3-C75E-406D-A7A7-2C27C91EA401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD6D5D7-360E-4322-888E-DD957919B3AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="23010" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -20,12 +20,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">schedule!$A$1:$N$19</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1332,22 +1331,22 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="9" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="9" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>12.38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>5</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>8</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>10</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>11</v>
       </c>
@@ -1764,7 +1763,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
         <v>12</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>11.71</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>10.44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>11.43</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="30">
         <v>17</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="32">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D18" s="32">
         <v>27</v>
@@ -1975,7 +1974,7 @@
         <v>9.41</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -2010,14 +2009,14 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="49" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="42">
         <f>SUM(C2:C19)</f>
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D20" s="42">
         <f>SUM(D2:D19)</f>
@@ -2025,7 +2024,7 @@
       </c>
       <c r="E20" s="49">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="43"/>
@@ -2059,26 +2058,26 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="71.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="45.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="92.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="140.6640625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="4"/>
-    <col min="10" max="10" width="52.44140625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="92.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="140.7109375" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" style="4"/>
+    <col min="10" max="10" width="52.42578125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2104,7 +2103,7 @@
         <v>&lt;a href="http://discuss.itversity.com/t/introduction-cca-175-spark-and-hadoop-developer-curriculum/19794" target="_blank"&gt;http://discuss.itversity.com/t/introduction-cca-175-spark-and-hadoop-developer-curriculum/19794&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2265,7 +2264,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2426,7 +2425,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2449,7 +2448,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2495,7 +2494,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2541,7 +2540,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2564,7 +2563,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2610,7 +2609,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -2679,7 +2678,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -2725,7 +2724,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2785,16 +2784,16 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="50.6640625" style="6"/>
+    <col min="1" max="1" width="49.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="50.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>13</v>
       </c>
@@ -2802,7 +2801,7 @@
       <c r="C1" s="51"/>
       <c r="D1" s="52"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>11</v>
       </c>
@@ -2840,7 +2839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -2854,8 +2853,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>42</v>
       </c>
@@ -2863,7 +2862,7 @@
       <c r="C8" s="56"/>
       <c r="D8" s="57"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -2877,7 +2876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -2891,7 +2890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -2905,7 +2904,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2919,7 +2918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2931,7 +2930,7 @@
       </c>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>37</v>
       </c>
@@ -2943,8 +2942,8 @@
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>43</v>
       </c>
@@ -2952,7 +2951,7 @@
       <c r="C17" s="56"/>
       <c r="D17" s="57"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -2960,7 +2959,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
chapter 17 - 6
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCodes\github\notes\cloudera1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD6D5D7-360E-4322-888E-DD957919B3AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1A579C-044C-4FA0-A950-BA478B7EB74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="23010" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -20,11 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">schedule!$A$1:$N$19</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -594,7 +595,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,12 +628,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -820,7 +815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -909,6 +904,15 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -918,28 +922,10 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -955,39 +941,36 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1331,22 +1314,22 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="9" width="8.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="9" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -1365,20 +1348,20 @@
       <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1398,22 +1381,22 @@
         <f>IF(C2=D2,"Completed",IF(C2=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H2" s="34">
-        <v>1</v>
-      </c>
-      <c r="I2" s="34">
+      <c r="H2" s="31">
+        <v>1</v>
+      </c>
+      <c r="I2" s="31">
         <v>6</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="31">
         <f t="shared" ref="J2:J9" si="0">H2*60+I2</f>
         <v>66</v>
       </c>
-      <c r="K2" s="40">
+      <c r="K2" s="37">
         <f t="shared" ref="K2:K9" si="1">ROUND(J2/D2,2)</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1433,22 +1416,22 @@
         <f t="shared" ref="F3:F9" si="2">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H3" s="34">
-        <v>1</v>
-      </c>
-      <c r="I3" s="34">
+      <c r="H3" s="31">
+        <v>1</v>
+      </c>
+      <c r="I3" s="31">
         <v>39</v>
       </c>
-      <c r="J3" s="34">
+      <c r="J3" s="31">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="K3" s="40">
+      <c r="K3" s="37">
         <f t="shared" si="1"/>
         <v>12.38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -1468,22 +1451,22 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H4" s="34">
-        <v>1</v>
-      </c>
-      <c r="I4" s="34">
+      <c r="H4" s="31">
+        <v>1</v>
+      </c>
+      <c r="I4" s="31">
         <v>33</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="31">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="K4" s="40">
+      <c r="K4" s="37">
         <f t="shared" si="1"/>
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -1503,22 +1486,22 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H5" s="34">
-        <v>0</v>
-      </c>
-      <c r="I5" s="34">
+      <c r="H5" s="31">
+        <v>0</v>
+      </c>
+      <c r="I5" s="31">
         <v>37</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="31">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K5" s="40">
+      <c r="K5" s="37">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>5</v>
       </c>
@@ -1538,22 +1521,22 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H6" s="34">
-        <v>0</v>
-      </c>
-      <c r="I6" s="34">
+      <c r="H6" s="31">
+        <v>0</v>
+      </c>
+      <c r="I6" s="31">
         <v>52</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="31">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="K6" s="40">
+      <c r="K6" s="37">
         <f t="shared" si="1"/>
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -1573,22 +1556,22 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H7" s="34">
-        <v>1</v>
-      </c>
-      <c r="I7" s="34">
+      <c r="H7" s="31">
+        <v>1</v>
+      </c>
+      <c r="I7" s="31">
         <v>14</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="31">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="37">
         <f t="shared" si="1"/>
         <v>5.29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -1608,22 +1591,22 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H8" s="34">
-        <v>0</v>
-      </c>
-      <c r="I8" s="34">
+      <c r="H8" s="31">
+        <v>0</v>
+      </c>
+      <c r="I8" s="31">
         <v>50</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="31">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="37">
         <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>8</v>
       </c>
@@ -1643,22 +1626,22 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H9" s="34">
-        <v>1</v>
-      </c>
-      <c r="I9" s="34">
+      <c r="H9" s="31">
+        <v>1</v>
+      </c>
+      <c r="I9" s="31">
         <v>16</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="31">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="37">
         <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -1678,22 +1661,22 @@
         <f t="shared" ref="F10:F19" si="3">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
         <v>Not Started</v>
       </c>
-      <c r="H10" s="34">
-        <v>0</v>
-      </c>
-      <c r="I10" s="34">
+      <c r="H10" s="31">
+        <v>0</v>
+      </c>
+      <c r="I10" s="31">
         <v>47</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="31">
         <f>H10*60+I10</f>
         <v>47</v>
       </c>
-      <c r="K10" s="41">
+      <c r="K10" s="38">
         <f>ROUND(J10/D10,2)</f>
         <v>3.62</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="27">
         <v>10</v>
       </c>
@@ -1713,22 +1696,22 @@
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="31">
         <v>5</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="31">
         <v>47</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="31">
         <f>H11*60+I11</f>
         <v>347</v>
       </c>
-      <c r="K11" s="40">
+      <c r="K11" s="37">
         <f t="shared" ref="K11:K18" si="4">ROUND(J11/D11,2)</f>
         <v>7.89</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <v>11</v>
       </c>
@@ -1748,57 +1731,57 @@
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H12" s="34">
-        <v>1</v>
-      </c>
-      <c r="I12" s="34">
+      <c r="H12" s="31">
+        <v>1</v>
+      </c>
+      <c r="I12" s="31">
         <v>35</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="31">
         <f t="shared" ref="J12:J19" si="5">H12*60+I12</f>
         <v>95</v>
       </c>
-      <c r="K12" s="40">
+      <c r="K12" s="37">
         <f t="shared" si="4"/>
         <v>7.92</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="33">
         <v>12</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="35">
         <v>21</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="35">
         <v>21</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="36" t="str">
+      <c r="F13" s="33" t="str">
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="31">
         <v>4</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="31">
         <v>6</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="31">
         <f t="shared" si="5"/>
         <v>246</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="37">
         <f t="shared" si="4"/>
         <v>11.71</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -1818,22 +1801,22 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H14" s="34">
-        <v>1</v>
-      </c>
-      <c r="I14" s="34">
+      <c r="H14" s="31">
+        <v>1</v>
+      </c>
+      <c r="I14" s="31">
         <v>34</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="31">
         <f t="shared" si="5"/>
         <v>94</v>
       </c>
-      <c r="K14" s="41">
+      <c r="K14" s="38">
         <f t="shared" si="4"/>
         <v>10.44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -1853,22 +1836,22 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H15" s="34">
-        <v>1</v>
-      </c>
-      <c r="I15" s="34">
+      <c r="H15" s="31">
+        <v>1</v>
+      </c>
+      <c r="I15" s="31">
         <v>12</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="31">
         <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="K15" s="41">
+      <c r="K15" s="38">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -1888,22 +1871,22 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H16" s="34">
-        <v>1</v>
-      </c>
-      <c r="I16" s="34">
+      <c r="H16" s="31">
+        <v>1</v>
+      </c>
+      <c r="I16" s="31">
         <v>20</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="31">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="K16" s="41">
+      <c r="K16" s="38">
         <f t="shared" si="4"/>
         <v>11.43</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -1923,58 +1906,58 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H17" s="34">
-        <v>0</v>
-      </c>
-      <c r="I17" s="34">
+      <c r="H17" s="31">
+        <v>0</v>
+      </c>
+      <c r="I17" s="31">
         <v>53</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="31">
         <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="K17" s="41">
+      <c r="K17" s="38">
         <f t="shared" si="4"/>
         <v>7.57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="33">
         <v>17</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="32">
-        <v>20</v>
-      </c>
-      <c r="D18" s="32">
+      <c r="C18" s="35">
         <v>27</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="D18" s="35">
+        <v>27</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="30" t="str">
+      <c r="F18" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>In Progress</v>
-      </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47">
+        <v>Completed</v>
+      </c>
+      <c r="G18" s="52"/>
+      <c r="H18" s="53">
         <v>4</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="53">
         <v>14</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="53">
         <f t="shared" si="5"/>
         <v>254</v>
       </c>
-      <c r="K18" s="48">
+      <c r="K18" s="37">
         <f t="shared" si="4"/>
         <v>9.41</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -1994,47 +1977,47 @@
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H19" s="34">
-        <v>1</v>
-      </c>
-      <c r="I19" s="34">
-        <v>0</v>
-      </c>
-      <c r="J19" s="34">
+      <c r="H19" s="31">
+        <v>1</v>
+      </c>
+      <c r="I19" s="31">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="K19" s="41">
+      <c r="K19" s="38">
         <f>ROUND(J19/D19,2)</f>
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="49" t="s">
+    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="42">
+      <c r="B20" s="43"/>
+      <c r="C20" s="39">
         <f>SUM(C2:C19)</f>
-        <v>190</v>
-      </c>
-      <c r="D20" s="42">
+        <v>197</v>
+      </c>
+      <c r="D20" s="39">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="43">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>76</v>
-      </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="44">
+        <v>79</v>
+      </c>
+      <c r="F20" s="43"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="41">
         <f>SUM(J2:J19)</f>
         <v>1895</v>
       </c>
-      <c r="K20" s="45">
+      <c r="K20" s="42">
         <f>ROUND(J20/D20,2)</f>
         <v>7.61</v>
       </c>
@@ -2058,26 +2041,26 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="2.28515625" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="92.7109375" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="140.7109375" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" style="4"/>
-    <col min="10" max="10" width="52.42578125" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="9.109375" style="4" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="2.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="45.109375" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="92.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="140.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="52.44140625" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2103,7 +2086,7 @@
         <v>&lt;a href="http://discuss.itversity.com/t/introduction-cca-175-spark-and-hadoop-developer-curriculum/19794" target="_blank"&gt;http://discuss.itversity.com/t/introduction-cca-175-spark-and-hadoop-developer-curriculum/19794&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2126,7 +2109,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2149,7 +2132,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2172,7 +2155,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2195,7 +2178,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2218,7 +2201,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2224,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2264,7 +2247,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2287,7 +2270,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2310,7 +2293,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2333,7 +2316,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2356,7 +2339,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2379,7 +2362,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2402,7 +2385,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2425,7 +2408,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2448,7 +2431,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2471,7 +2454,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2494,7 +2477,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2517,7 +2500,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2540,7 +2523,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2563,7 +2546,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2586,7 +2569,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2609,7 +2592,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -2632,7 +2615,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2655,7 +2638,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -2678,7 +2661,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2701,7 +2684,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -2724,7 +2707,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2747,7 +2730,7 @@
         <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2784,24 +2767,24 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="50.7109375" style="6"/>
+    <col min="1" max="1" width="49.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="50.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="46"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2815,7 +2798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
@@ -2829,17 +2812,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -2853,16 +2836,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
+    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="45"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -2876,7 +2859,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -2890,7 +2873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -2904,7 +2887,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2918,7 +2901,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2930,7 +2913,7 @@
       </c>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="192" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>37</v>
       </c>
@@ -2942,16 +2925,16 @@
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+    <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="45"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -2959,7 +2942,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:4" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
chapter 13 - 1
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1A579C-044C-4FA0-A950-BA478B7EB74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F4F4A3-687E-4DC5-97B3-F39A9D691F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -595,7 +595,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +632,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -815,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -941,36 +947,52 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1314,7 +1336,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1782,36 +1804,37 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+      <c r="A14" s="45">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="25">
-        <v>0</v>
-      </c>
-      <c r="D14" s="25">
+      <c r="C14" s="47">
+        <v>7</v>
+      </c>
+      <c r="D14" s="47">
         <v>9</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="23" t="str">
+      <c r="F14" s="45" t="str">
         <f t="shared" si="3"/>
-        <v>Not Started</v>
-      </c>
-      <c r="H14" s="31">
-        <v>1</v>
-      </c>
-      <c r="I14" s="31">
+        <v>In Progress</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49">
+        <v>1</v>
+      </c>
+      <c r="I14" s="49">
         <v>34</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="49">
         <f t="shared" si="5"/>
         <v>94</v>
       </c>
-      <c r="K14" s="38">
+      <c r="K14" s="50">
         <f t="shared" si="4"/>
         <v>10.44</v>
       </c>
@@ -1941,14 +1964,14 @@
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53">
+      <c r="G18" s="43"/>
+      <c r="H18" s="44">
         <v>4</v>
       </c>
-      <c r="I18" s="53">
+      <c r="I18" s="44">
         <v>14</v>
       </c>
-      <c r="J18" s="53">
+      <c r="J18" s="44">
         <f t="shared" si="5"/>
         <v>254</v>
       </c>
@@ -1993,23 +2016,23 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="43"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="39">
         <f>SUM(C2:C19)</f>
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D20" s="39">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="51">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>79</v>
-      </c>
-      <c r="F20" s="43"/>
+        <v>82</v>
+      </c>
+      <c r="F20" s="51"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
@@ -2777,12 +2800,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2813,11 +2836,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2838,12 +2861,12 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -2927,12 +2950,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>

<commit_message>
chapter 14 - 1
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F4F4A3-687E-4DC5-97B3-F39A9D691F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89999463-52A7-4740-991E-8C5202059806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -821,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -901,15 +901,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -917,15 +908,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -947,23 +929,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -993,6 +958,54 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1336,7 +1349,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,16 +1383,16 @@
       <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="30" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1403,17 +1416,17 @@
         <f>IF(C2=D2,"Completed",IF(C2=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H2" s="31">
-        <v>1</v>
-      </c>
-      <c r="I2" s="31">
+      <c r="H2" s="28">
+        <v>1</v>
+      </c>
+      <c r="I2" s="28">
         <v>6</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="28">
         <f t="shared" ref="J2:J9" si="0">H2*60+I2</f>
         <v>66</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="31">
         <f t="shared" ref="K2:K9" si="1">ROUND(J2/D2,2)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -1438,17 +1451,17 @@
         <f t="shared" ref="F3:F9" si="2">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H3" s="31">
-        <v>1</v>
-      </c>
-      <c r="I3" s="31">
+      <c r="H3" s="28">
+        <v>1</v>
+      </c>
+      <c r="I3" s="28">
         <v>39</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="28">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="31">
         <f t="shared" si="1"/>
         <v>12.38</v>
       </c>
@@ -1473,17 +1486,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H4" s="31">
-        <v>1</v>
-      </c>
-      <c r="I4" s="31">
+      <c r="H4" s="28">
+        <v>1</v>
+      </c>
+      <c r="I4" s="28">
         <v>33</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="28">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="31">
         <f t="shared" si="1"/>
         <v>9.3000000000000007</v>
       </c>
@@ -1508,17 +1521,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H5" s="31">
-        <v>0</v>
-      </c>
-      <c r="I5" s="31">
+      <c r="H5" s="28">
+        <v>0</v>
+      </c>
+      <c r="I5" s="28">
         <v>37</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="28">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="31">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
@@ -1543,17 +1556,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H6" s="31">
-        <v>0</v>
-      </c>
-      <c r="I6" s="31">
+      <c r="H6" s="28">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
         <v>52</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="28">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="31">
         <f t="shared" si="1"/>
         <v>4.7300000000000004</v>
       </c>
@@ -1578,17 +1591,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H7" s="31">
-        <v>1</v>
-      </c>
-      <c r="I7" s="31">
+      <c r="H7" s="28">
+        <v>1</v>
+      </c>
+      <c r="I7" s="28">
         <v>14</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="28">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="31">
         <f t="shared" si="1"/>
         <v>5.29</v>
       </c>
@@ -1613,17 +1626,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H8" s="31">
-        <v>0</v>
-      </c>
-      <c r="I8" s="31">
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28">
         <v>50</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="28">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="31">
         <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
@@ -1648,17 +1661,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H9" s="31">
-        <v>1</v>
-      </c>
-      <c r="I9" s="31">
+      <c r="H9" s="28">
+        <v>1</v>
+      </c>
+      <c r="I9" s="28">
         <v>16</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="28">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="31">
         <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
@@ -1683,364 +1696,371 @@
         <f t="shared" ref="F10:F19" si="3">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
         <v>Not Started</v>
       </c>
-      <c r="H10" s="31">
-        <v>0</v>
-      </c>
-      <c r="I10" s="31">
+      <c r="H10" s="28">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28">
         <v>47</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="28">
         <f>H10*60+I10</f>
         <v>47</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="32">
         <f>ROUND(J10/D10,2)</f>
         <v>3.62</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
+      <c r="A11" s="47">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="49">
         <v>44</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="49">
         <v>44</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="27" t="str">
+      <c r="F11" s="47" t="str">
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H11" s="31">
+      <c r="G11" s="50"/>
+      <c r="H11" s="51">
         <v>5</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="51">
         <v>47</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="51">
         <f>H11*60+I11</f>
         <v>347</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="31">
         <f t="shared" ref="K11:K18" si="4">ROUND(J11/D11,2)</f>
         <v>7.89</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
+      <c r="A12" s="47">
         <v>11</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="49">
         <v>12</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="49">
         <v>12</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="20" t="str">
+      <c r="F12" s="47" t="str">
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H12" s="31">
-        <v>1</v>
-      </c>
-      <c r="I12" s="31">
+      <c r="G12" s="50"/>
+      <c r="H12" s="51">
+        <v>1</v>
+      </c>
+      <c r="I12" s="51">
         <v>35</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="51">
         <f t="shared" ref="J12:J19" si="5">H12*60+I12</f>
         <v>95</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="31">
         <f t="shared" si="4"/>
         <v>7.92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="33">
+      <c r="A13" s="52">
         <v>12</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="54">
         <v>21</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="54">
         <v>21</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="33" t="str">
+      <c r="F13" s="52" t="str">
         <f t="shared" si="3"/>
         <v>Completed</v>
       </c>
-      <c r="H13" s="31">
+      <c r="G13" s="50"/>
+      <c r="H13" s="51">
         <v>4</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="51">
         <v>6</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="51">
         <f t="shared" si="5"/>
         <v>246</v>
       </c>
-      <c r="K13" s="37">
+      <c r="K13" s="31">
         <f t="shared" si="4"/>
         <v>11.71</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="45">
+      <c r="A14" s="52">
         <v>13</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="47">
-        <v>7</v>
-      </c>
-      <c r="D14" s="47">
+      <c r="C14" s="54">
         <v>9</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="D14" s="54">
+        <v>9</v>
+      </c>
+      <c r="E14" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="45" t="str">
+      <c r="F14" s="52" t="str">
+        <f t="shared" si="3"/>
+        <v>Completed</v>
+      </c>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56">
+        <v>1</v>
+      </c>
+      <c r="I14" s="56">
+        <v>34</v>
+      </c>
+      <c r="J14" s="56">
+        <f t="shared" si="5"/>
+        <v>94</v>
+      </c>
+      <c r="K14" s="31">
+        <f t="shared" si="4"/>
+        <v>10.44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="57">
+        <v>14</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="59">
+        <v>2</v>
+      </c>
+      <c r="D15" s="59">
+        <v>8</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="57" t="str">
         <f t="shared" si="3"/>
         <v>In Progress</v>
       </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49">
-        <v>1</v>
-      </c>
-      <c r="I14" s="49">
-        <v>34</v>
-      </c>
-      <c r="J14" s="49">
+      <c r="G15" s="60"/>
+      <c r="H15" s="61">
+        <v>1</v>
+      </c>
+      <c r="I15" s="61">
+        <v>12</v>
+      </c>
+      <c r="J15" s="61">
         <f t="shared" si="5"/>
-        <v>94</v>
-      </c>
-      <c r="K14" s="50">
+        <v>72</v>
+      </c>
+      <c r="K15" s="37">
         <f t="shared" si="4"/>
-        <v>10.44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
-        <v>14</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="25">
-        <v>0</v>
-      </c>
-      <c r="D15" s="25">
-        <v>8</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="23" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="62">
+        <v>15</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="64">
+        <v>0</v>
+      </c>
+      <c r="D16" s="64">
+        <v>7</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="62" t="str">
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H15" s="31">
-        <v>1</v>
-      </c>
-      <c r="I15" s="31">
-        <v>12</v>
-      </c>
-      <c r="J15" s="31">
+      <c r="G16" s="50"/>
+      <c r="H16" s="51">
+        <v>1</v>
+      </c>
+      <c r="I16" s="51">
+        <v>20</v>
+      </c>
+      <c r="J16" s="51">
         <f t="shared" si="5"/>
-        <v>72</v>
-      </c>
-      <c r="K15" s="38">
+        <v>80</v>
+      </c>
+      <c r="K16" s="32">
         <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
-        <v>15</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="25">
-        <v>0</v>
-      </c>
-      <c r="D16" s="25">
+        <v>11.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="62">
+        <v>16</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="64">
+        <v>0</v>
+      </c>
+      <c r="D17" s="64">
         <v>7</v>
       </c>
-      <c r="E16" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="23" t="str">
+      <c r="E17" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="62" t="str">
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H16" s="31">
-        <v>1</v>
-      </c>
-      <c r="I16" s="31">
-        <v>20</v>
-      </c>
-      <c r="J16" s="31">
+      <c r="G17" s="50"/>
+      <c r="H17" s="51">
+        <v>0</v>
+      </c>
+      <c r="I17" s="51">
+        <v>53</v>
+      </c>
+      <c r="J17" s="51">
         <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="K16" s="38">
+        <v>53</v>
+      </c>
+      <c r="K17" s="32">
         <f t="shared" si="4"/>
-        <v>11.43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
-        <v>16</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="25">
-        <v>0</v>
-      </c>
-      <c r="D17" s="25">
-        <v>7</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="23" t="str">
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="52">
+        <v>17</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="54">
+        <v>27</v>
+      </c>
+      <c r="D18" s="54">
+        <v>27</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="52" t="str">
+        <f t="shared" si="3"/>
+        <v>Completed</v>
+      </c>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56">
+        <v>4</v>
+      </c>
+      <c r="I18" s="56">
+        <v>14</v>
+      </c>
+      <c r="J18" s="56">
+        <f t="shared" si="5"/>
+        <v>254</v>
+      </c>
+      <c r="K18" s="31">
+        <f t="shared" si="4"/>
+        <v>9.41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="62">
+        <v>18</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="64">
+        <v>0</v>
+      </c>
+      <c r="D19" s="64">
+        <v>8</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="62" t="str">
         <f t="shared" si="3"/>
         <v>Not Started</v>
       </c>
-      <c r="H17" s="31">
-        <v>0</v>
-      </c>
-      <c r="I17" s="31">
-        <v>53</v>
-      </c>
-      <c r="J17" s="31">
-        <f t="shared" si="5"/>
-        <v>53</v>
-      </c>
-      <c r="K17" s="38">
-        <f t="shared" si="4"/>
-        <v>7.57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="33">
-        <v>17</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="35">
-        <v>27</v>
-      </c>
-      <c r="D18" s="35">
-        <v>27</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="33" t="str">
-        <f t="shared" si="3"/>
-        <v>Completed</v>
-      </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44">
-        <v>4</v>
-      </c>
-      <c r="I18" s="44">
-        <v>14</v>
-      </c>
-      <c r="J18" s="44">
-        <f t="shared" si="5"/>
-        <v>254</v>
-      </c>
-      <c r="K18" s="37">
-        <f t="shared" si="4"/>
-        <v>9.41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>18</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="25">
-        <v>0</v>
-      </c>
-      <c r="D19" s="25">
-        <v>8</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="23" t="str">
-        <f t="shared" si="3"/>
-        <v>Not Started</v>
-      </c>
-      <c r="H19" s="31">
-        <v>1</v>
-      </c>
-      <c r="I19" s="31">
-        <v>0</v>
-      </c>
-      <c r="J19" s="31">
+      <c r="G19" s="50"/>
+      <c r="H19" s="51">
+        <v>1</v>
+      </c>
+      <c r="I19" s="51">
+        <v>0</v>
+      </c>
+      <c r="J19" s="51">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="32">
         <f>ROUND(J19/D19,2)</f>
         <v>7.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="39">
+      <c r="B20" s="38"/>
+      <c r="C20" s="33">
         <f>SUM(C2:C19)</f>
-        <v>204</v>
-      </c>
-      <c r="D20" s="39">
+        <v>208</v>
+      </c>
+      <c r="D20" s="33">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="38">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>82</v>
-      </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="41">
+        <v>84</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="35">
         <f>SUM(J2:J19)</f>
         <v>1895</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="36">
         <f>ROUND(J20/D20,2)</f>
         <v>7.61</v>
       </c>
@@ -2800,12 +2820,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2836,11 +2856,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2861,12 +2881,12 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -2950,12 +2970,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>

<commit_message>
Chapter 18 - 1
</commit_message>
<xml_diff>
--- a/cloudera1/link-template.xlsx
+++ b/cloudera1/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\cloudera1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE25850-FAEA-41E1-9B47-E56081098044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88032733-EE4B-4E78-8475-C96B9D4202EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,19 +631,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,7 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -924,15 +918,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -946,9 +931,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,9 +946,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -980,6 +959,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -993,54 +1021,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1384,7 +1366,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,37 +1392,37 @@
       <c r="B1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="43" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1464,17 +1446,17 @@
         <f>IF(C2=D2,"Completed",IF(C2=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H2" s="28">
-        <v>1</v>
-      </c>
-      <c r="I2" s="28">
+      <c r="H2" s="25">
+        <v>1</v>
+      </c>
+      <c r="I2" s="25">
         <v>6</v>
       </c>
-      <c r="J2" s="28">
+      <c r="J2" s="25">
         <f t="shared" ref="J2:J9" si="0">H2*60+I2</f>
         <v>66</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="28">
         <f t="shared" ref="K2:K9" si="1">ROUND(J2/D2,2)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -1510,17 +1492,17 @@
         <f t="shared" ref="F3:F9" si="2">IF(C3=D3,"Completed",IF(C3=0,"Not Started","In Progress"))</f>
         <v>Completed</v>
       </c>
-      <c r="H3" s="28">
-        <v>1</v>
-      </c>
-      <c r="I3" s="28">
+      <c r="H3" s="25">
+        <v>1</v>
+      </c>
+      <c r="I3" s="25">
         <v>39</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="25">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="28">
         <f t="shared" si="1"/>
         <v>12.38</v>
       </c>
@@ -1556,17 +1538,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H4" s="28">
-        <v>1</v>
-      </c>
-      <c r="I4" s="28">
+      <c r="H4" s="25">
+        <v>1</v>
+      </c>
+      <c r="I4" s="25">
         <v>33</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="25">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="28">
         <f t="shared" si="1"/>
         <v>9.3000000000000007</v>
       </c>
@@ -1602,17 +1584,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H5" s="28">
-        <v>0</v>
-      </c>
-      <c r="I5" s="28">
+      <c r="H5" s="25">
+        <v>0</v>
+      </c>
+      <c r="I5" s="25">
         <v>37</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="25">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="28">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
@@ -1648,17 +1630,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H6" s="28">
-        <v>0</v>
-      </c>
-      <c r="I6" s="28">
+      <c r="H6" s="25">
+        <v>0</v>
+      </c>
+      <c r="I6" s="25">
         <v>52</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="25">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="28">
         <f t="shared" si="1"/>
         <v>4.7300000000000004</v>
       </c>
@@ -1694,17 +1676,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H7" s="28">
-        <v>1</v>
-      </c>
-      <c r="I7" s="28">
+      <c r="H7" s="25">
+        <v>1</v>
+      </c>
+      <c r="I7" s="25">
         <v>14</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="25">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="28">
         <f t="shared" si="1"/>
         <v>5.29</v>
       </c>
@@ -1740,17 +1722,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H8" s="28">
-        <v>0</v>
-      </c>
-      <c r="I8" s="28">
+      <c r="H8" s="25">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25">
         <v>50</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="25">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="28">
         <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
@@ -1786,17 +1768,17 @@
         <f t="shared" si="2"/>
         <v>Completed</v>
       </c>
-      <c r="H9" s="28">
-        <v>1</v>
-      </c>
-      <c r="I9" s="28">
+      <c r="H9" s="25">
+        <v>1</v>
+      </c>
+      <c r="I9" s="25">
         <v>16</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="25">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="28">
         <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
@@ -1813,87 +1795,87 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="23">
+      <c r="A10" s="20">
         <v>9</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="25">
-        <v>0</v>
-      </c>
-      <c r="D10" s="25">
+      <c r="C10" s="22">
         <v>13</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="22">
+        <v>13</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="23" t="str">
+      <c r="F10" s="20" t="str">
         <f t="shared" ref="F10:F19" si="5">IF(C10=D10,"Completed",IF(C10=0,"Not Started","In Progress"))</f>
-        <v>Not Started</v>
-      </c>
-      <c r="H10" s="28">
-        <v>0</v>
-      </c>
-      <c r="I10" s="28">
+        <v>Completed</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25">
         <v>47</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="25">
         <f>H10*60+I10</f>
         <v>47</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="28">
         <f>ROUND(J10/D10,2)</f>
         <v>3.62</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="20">
         <v>47</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="23">
+        <v>611</v>
+      </c>
+      <c r="N10" s="20">
         <f t="shared" si="4"/>
         <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
+      <c r="A11" s="33">
         <v>10</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="35">
         <v>44</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="35">
         <v>44</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="38" t="str">
+      <c r="F11" s="33" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42">
+      <c r="G11" s="36"/>
+      <c r="H11" s="37">
         <v>5</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="37">
         <v>47</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="37">
         <f>H11*60+I11</f>
         <v>347</v>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="28">
         <f t="shared" ref="K11:K18" si="6">ROUND(J11/D11,2)</f>
         <v>7.89</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="33">
         <v>347</v>
       </c>
       <c r="M11" s="20">
@@ -1906,41 +1888,41 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="38">
+      <c r="A12" s="33">
         <v>11</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="35">
         <v>12</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="35">
         <v>12</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="38" t="str">
+      <c r="F12" s="33" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42">
-        <v>1</v>
-      </c>
-      <c r="I12" s="42">
+      <c r="G12" s="36"/>
+      <c r="H12" s="37">
+        <v>1</v>
+      </c>
+      <c r="I12" s="37">
         <v>35</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="37">
         <f t="shared" ref="J12:J19" si="7">H12*60+I12</f>
         <v>95</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="28">
         <f t="shared" si="6"/>
         <v>7.92</v>
       </c>
-      <c r="L12" s="38">
+      <c r="L12" s="33">
         <v>95</v>
       </c>
       <c r="M12" s="20">
@@ -1953,41 +1935,41 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="43">
+      <c r="A13" s="38">
         <v>12</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="40">
         <v>21</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="40">
         <v>21</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="43" t="str">
+      <c r="F13" s="38" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42">
+      <c r="G13" s="36"/>
+      <c r="H13" s="37">
         <v>4</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="37">
         <v>6</v>
       </c>
-      <c r="J13" s="42">
+      <c r="J13" s="37">
         <f t="shared" si="7"/>
         <v>246</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="28">
         <f t="shared" si="6"/>
         <v>11.71</v>
       </c>
-      <c r="L13" s="43">
+      <c r="L13" s="38">
         <v>246</v>
       </c>
       <c r="M13" s="20">
@@ -2000,41 +1982,41 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="43">
+      <c r="A14" s="38">
         <v>13</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="40">
         <v>9</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="40">
         <v>9</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="43" t="str">
+      <c r="F14" s="38" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47">
-        <v>1</v>
-      </c>
-      <c r="I14" s="47">
+      <c r="G14" s="41"/>
+      <c r="H14" s="42">
+        <v>1</v>
+      </c>
+      <c r="I14" s="42">
         <v>34</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="42">
         <f t="shared" si="7"/>
         <v>94</v>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="28">
         <f t="shared" si="6"/>
         <v>10.44</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="38">
         <v>94</v>
       </c>
       <c r="M14" s="20">
@@ -2047,41 +2029,41 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="43">
+      <c r="A15" s="38">
         <v>14</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="40">
         <v>8</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="40">
         <v>8</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="43" t="str">
+      <c r="F15" s="38" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="47">
-        <v>1</v>
-      </c>
-      <c r="I15" s="47">
+      <c r="G15" s="41"/>
+      <c r="H15" s="42">
+        <v>1</v>
+      </c>
+      <c r="I15" s="42">
         <v>12</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="42">
         <f t="shared" si="7"/>
         <v>72</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="28">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="38">
         <v>72</v>
       </c>
       <c r="M15" s="20">
@@ -2094,135 +2076,135 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="43">
+      <c r="A16" s="38">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="40">
         <v>7</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="40">
         <v>7</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="43" t="str">
+      <c r="F16" s="38" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47">
-        <v>1</v>
-      </c>
-      <c r="I16" s="47">
+      <c r="G16" s="41"/>
+      <c r="H16" s="42">
+        <v>1</v>
+      </c>
+      <c r="I16" s="42">
         <v>20</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="42">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="28">
         <f t="shared" si="6"/>
         <v>11.43</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L16" s="38">
         <v>80</v>
       </c>
-      <c r="M16" s="43">
+      <c r="M16" s="38">
         <f t="shared" si="3"/>
         <v>560</v>
       </c>
-      <c r="N16" s="43">
+      <c r="N16" s="38">
         <f t="shared" si="4"/>
         <v>560</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="43">
+      <c r="A17" s="38">
         <v>16</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="40">
         <v>7</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="40">
         <v>7</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="43" t="str">
+      <c r="F17" s="38" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="47">
-        <v>0</v>
-      </c>
-      <c r="I17" s="47">
+      <c r="G17" s="41"/>
+      <c r="H17" s="42">
+        <v>0</v>
+      </c>
+      <c r="I17" s="42">
         <v>53</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="42">
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="28">
         <f t="shared" si="6"/>
         <v>7.57</v>
       </c>
-      <c r="L17" s="43">
+      <c r="L17" s="38">
         <v>53</v>
       </c>
-      <c r="M17" s="43">
+      <c r="M17" s="38">
         <f t="shared" si="3"/>
         <v>371</v>
       </c>
-      <c r="N17" s="43">
+      <c r="N17" s="38">
         <f t="shared" si="4"/>
         <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="43">
+      <c r="A18" s="38">
         <v>17</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="40">
         <v>27</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="40">
         <v>27</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="43" t="str">
+      <c r="F18" s="38" t="str">
         <f t="shared" si="5"/>
         <v>Completed</v>
       </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47">
+      <c r="G18" s="41"/>
+      <c r="H18" s="42">
         <v>4</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="42">
         <v>14</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="42">
         <f t="shared" si="7"/>
         <v>254</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="28">
         <f t="shared" si="6"/>
         <v>9.41</v>
       </c>
-      <c r="L18" s="43">
+      <c r="L18" s="38">
         <v>254</v>
       </c>
       <c r="M18" s="20">
@@ -2235,86 +2217,86 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="48">
+      <c r="A19" s="55">
         <v>18</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="50">
-        <v>1</v>
-      </c>
-      <c r="D19" s="50">
+      <c r="C19" s="57">
+        <v>2</v>
+      </c>
+      <c r="D19" s="57">
         <v>8</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="48" t="str">
+      <c r="F19" s="55" t="str">
         <f t="shared" si="5"/>
         <v>In Progress</v>
       </c>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52">
-        <v>1</v>
-      </c>
-      <c r="I19" s="52">
-        <v>0</v>
-      </c>
-      <c r="J19" s="52">
+      <c r="G19" s="58"/>
+      <c r="H19" s="59">
+        <v>1</v>
+      </c>
+      <c r="I19" s="59">
+        <v>0</v>
+      </c>
+      <c r="J19" s="59">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="K19" s="37">
+      <c r="K19" s="60">
         <f>ROUND(J19/D19,2)</f>
         <v>7.5</v>
       </c>
-      <c r="L19" s="48">
+      <c r="L19" s="55">
         <v>60</v>
       </c>
-      <c r="M19" s="48">
+      <c r="M19" s="55">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="N19" s="48">
+        <v>120</v>
+      </c>
+      <c r="N19" s="55">
         <f t="shared" si="4"/>
         <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="33">
+      <c r="B20" s="44"/>
+      <c r="C20" s="29">
         <f>SUM(C2:C19)</f>
-        <v>229</v>
-      </c>
-      <c r="D20" s="33">
+        <v>243</v>
+      </c>
+      <c r="D20" s="29">
         <f>SUM(D2:D19)</f>
         <v>249</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="44">
         <f>ROUND(C20*100/D20,0)</f>
-        <v>92</v>
-      </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35">
+        <v>98</v>
+      </c>
+      <c r="F20" s="44"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31">
         <f>SUM(J2:J19)</f>
         <v>1895</v>
       </c>
-      <c r="K20" s="36">
+      <c r="K20" s="32">
         <f>ROUND(J20/D20,2)</f>
         <v>7.61</v>
       </c>
-      <c r="M20" s="55">
+      <c r="M20" s="45">
         <f>ROUND((SUM(M2:M19)/SUM(N2:N19)*100),2)</f>
-        <v>97.3</v>
-      </c>
-      <c r="N20" s="56"/>
+        <v>99.06</v>
+      </c>
+      <c r="N20" s="46"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N19" xr:uid="{D3CEC666-E820-4D85-92B5-084C9F56284E}"/>
@@ -3072,12 +3054,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -3108,11 +3090,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
@@ -3133,12 +3115,12 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -3222,12 +3204,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">

</xml_diff>